<commit_message>
Update: 1) added RAW data for artropods 2) change most figures to half violins 3) adjusted models accordingly
</commit_message>
<xml_diff>
--- a/data/input/INV_clean.xlsx
+++ b/data/input/INV_clean.xlsx
@@ -8,16 +8,15 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ondre\Documents\HOPE\GITHUB\PNG-Ecxlosure\data\input\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B6A6699E-D591-4BCD-BB84-C2819CBF592F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5E8118D5-9B52-4EE2-9C74-A5C2AA7E47F8}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{5D0F1FD3-29CA-4560-9371-7370040DA6DC}"/>
+    <workbookView xWindow="28680" yWindow="-90" windowWidth="29040" windowHeight="15840" xr2:uid="{5D0F1FD3-29CA-4560-9371-7370040DA6DC}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
-    <sheet name="INV_clean (2)" sheetId="2" r:id="rId2"/>
+    <sheet name="INV_clean (2)" sheetId="2" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">'INV_clean (2)'!$A$1:$I$2342</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'INV_clean (2)'!$A$1:$I$2342</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -553,18 +552,6 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CC7C53F1-5F2A-4623-9C0F-051676B9AEB9}">
-  <dimension ref="A1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2D04BA6F-165F-4A87-A7A4-914E98075E04}">
   <dimension ref="A1:T2342"/>
   <sheetViews>
@@ -73209,9 +73196,12 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
@@ -73347,26 +73337,15 @@
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{50417D51-23A4-4991-BA20-093E80774A27}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{784D1462-B92A-4240-933A-3D45C028DD54}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="c96ed439-3b39-4220-95f1-971e18625870"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
@@ -73390,9 +73369,17 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{784D1462-B92A-4240-933A-3D45C028DD54}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{50417D51-23A4-4991-BA20-093E80774A27}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="c96ed439-3b39-4220-95f1-971e18625870"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>